<commit_message>
Create Tree,Generate data by the tree,Use sklear to predict and get the accurcy
</commit_message>
<xml_diff>
--- a/HW_2/DM_HW2_filted.xlsx
+++ b/HW_2/DM_HW2_filted.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syushengwei/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syushengwei/Desktop/2017-DataMining/HW_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,14 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>人因工程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>線性代數</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>模擬導論</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,14 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>企業通訊網路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>java 網路應用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>離散數學</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>心理學</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>策略管理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -90,28 +70,45 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>服務管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>策略定價</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>管理數學</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>領導學</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>雲端行動應用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Management Math</t>
+  </si>
+  <si>
+    <t>Human Factors Engineering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cloud Mobile Applications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer Network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psychology</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>Service Management</t>
   </si>
 </sst>
 </file>
@@ -448,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -474,7 +471,7 @@
   <sheetData>
     <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -486,58 +483,58 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.15">
@@ -1033,6 +1030,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="E13">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>45</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="N13">
+        <v>30</v>
+      </c>
+      <c r="Q13">
+        <v>30</v>
+      </c>
+      <c r="R13">
+        <v>45</v>
+      </c>
+      <c r="U13">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>